<commit_message>
Added some new files to repo
</commit_message>
<xml_diff>
--- a/Week5/mcnulty/mushroom_table.xlsx
+++ b/Week5/mcnulty/mushroom_table.xlsx
@@ -8,13 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bwsturm/ds/metis/metisbc/Week5/mcnulty/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6EC17DBE-E269-1945-A8B3-40902BBAE61B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{18270784-7199-224E-813E-E065D2DD8175}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10180" yWindow="1000" windowWidth="28040" windowHeight="17440" xr2:uid="{BC0C050D-CA9F-7344-8F13-F7CDCFE1754E}"/>
+    <workbookView xWindow="3600" yWindow="3180" windowWidth="28040" windowHeight="16660" activeTab="2" xr2:uid="{BC0C050D-CA9F-7344-8F13-F7CDCFE1754E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="logreg_coef" localSheetId="2">Sheet3!$A$2:$B$118</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,8 +29,21 @@
 </workbook>
 </file>
 
+<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{3689140A-1CD7-4D4E-9F6C-705F6305301C}" name="logreg_coef" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr codePage="10000" sourceFile="/Users/bwsturm/ds/metis/metisbc/Week5/mcnulty/logreg_coef.csv" comma="1">
+      <textFields count="2">
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+</connections>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="162">
   <si>
     <t>Mushroom ID table</t>
   </si>
@@ -79,13 +97,445 @@
   </si>
   <si>
     <t>ring</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cap-shape </t>
+  </si>
+  <si>
+    <t>Cap-surface</t>
+  </si>
+  <si>
+    <t>Cap-color </t>
+  </si>
+  <si>
+    <t>Odor </t>
+  </si>
+  <si>
+    <t>Bruises? </t>
+  </si>
+  <si>
+    <t>Spore-print-color </t>
+  </si>
+  <si>
+    <t>Population </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gill-attachment </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gill-spacing </t>
+  </si>
+  <si>
+    <t>Gill-size  </t>
+  </si>
+  <si>
+    <t>Gill-color</t>
+  </si>
+  <si>
+    <t>Stalk-shape  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stalk-root </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stalk-surface-above-ring </t>
+  </si>
+  <si>
+    <t>Stalk-surface-below-ring</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stalk-color-above-ring </t>
+  </si>
+  <si>
+    <t>Stalk-color-below-ring </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Veil-type </t>
+  </si>
+  <si>
+    <t>Veil-color </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ring-number </t>
+  </si>
+  <si>
+    <t>Ring-type </t>
+  </si>
+  <si>
+    <t>Habitat </t>
+  </si>
+  <si>
+    <t>Target</t>
+  </si>
+  <si>
+    <t>Poisonous</t>
+  </si>
+  <si>
+    <t>Edible</t>
+  </si>
+  <si>
+    <t>Feature</t>
+  </si>
+  <si>
+    <t>Beta</t>
+  </si>
+  <si>
+    <t>cap-shape_b</t>
+  </si>
+  <si>
+    <t>cap-shape_c</t>
+  </si>
+  <si>
+    <t>cap-shape_f</t>
+  </si>
+  <si>
+    <t>cap-shape_k</t>
+  </si>
+  <si>
+    <t>cap-shape_s</t>
+  </si>
+  <si>
+    <t>cap-shape_x</t>
+  </si>
+  <si>
+    <t>cap-surface_f</t>
+  </si>
+  <si>
+    <t>cap-surface_g</t>
+  </si>
+  <si>
+    <t>cap-surface_s</t>
+  </si>
+  <si>
+    <t>cap-surface_y</t>
+  </si>
+  <si>
+    <t>cap-color_b</t>
+  </si>
+  <si>
+    <t>cap-color_c</t>
+  </si>
+  <si>
+    <t>cap-color_e</t>
+  </si>
+  <si>
+    <t>cap-color_g</t>
+  </si>
+  <si>
+    <t>cap-color_n</t>
+  </si>
+  <si>
+    <t>cap-color_p</t>
+  </si>
+  <si>
+    <t>cap-color_r</t>
+  </si>
+  <si>
+    <t>cap-color_u</t>
+  </si>
+  <si>
+    <t>cap-color_w</t>
+  </si>
+  <si>
+    <t>cap-color_y</t>
+  </si>
+  <si>
+    <t>bruises_f</t>
+  </si>
+  <si>
+    <t>bruises_t</t>
+  </si>
+  <si>
+    <t>odor_a</t>
+  </si>
+  <si>
+    <t>odor_c</t>
+  </si>
+  <si>
+    <t>odor_f</t>
+  </si>
+  <si>
+    <t>odor_l</t>
+  </si>
+  <si>
+    <t>odor_m</t>
+  </si>
+  <si>
+    <t>odor_n</t>
+  </si>
+  <si>
+    <t>odor_p</t>
+  </si>
+  <si>
+    <t>odor_s</t>
+  </si>
+  <si>
+    <t>odor_y</t>
+  </si>
+  <si>
+    <t>gill-attachment_a</t>
+  </si>
+  <si>
+    <t>gill-attachment_f</t>
+  </si>
+  <si>
+    <t>gill-spacing_c</t>
+  </si>
+  <si>
+    <t>gill-spacing_w</t>
+  </si>
+  <si>
+    <t>gill-size_b</t>
+  </si>
+  <si>
+    <t>gill-size_n</t>
+  </si>
+  <si>
+    <t>gill-color_b</t>
+  </si>
+  <si>
+    <t>gill-color_e</t>
+  </si>
+  <si>
+    <t>gill-color_g</t>
+  </si>
+  <si>
+    <t>gill-color_h</t>
+  </si>
+  <si>
+    <t>gill-color_k</t>
+  </si>
+  <si>
+    <t>gill-color_n</t>
+  </si>
+  <si>
+    <t>gill-color_o</t>
+  </si>
+  <si>
+    <t>gill-color_p</t>
+  </si>
+  <si>
+    <t>gill-color_r</t>
+  </si>
+  <si>
+    <t>gill-color_u</t>
+  </si>
+  <si>
+    <t>gill-color_w</t>
+  </si>
+  <si>
+    <t>gill-color_y</t>
+  </si>
+  <si>
+    <t>stalk-shape_e</t>
+  </si>
+  <si>
+    <t>stalk-shape_t</t>
+  </si>
+  <si>
+    <t>stalk-root_?</t>
+  </si>
+  <si>
+    <t>stalk-root_b</t>
+  </si>
+  <si>
+    <t>stalk-root_c</t>
+  </si>
+  <si>
+    <t>stalk-root_e</t>
+  </si>
+  <si>
+    <t>stalk-root_r</t>
+  </si>
+  <si>
+    <t>stalk-surface-above-ring_f</t>
+  </si>
+  <si>
+    <t>stalk-surface-above-ring_k</t>
+  </si>
+  <si>
+    <t>stalk-surface-above-ring_s</t>
+  </si>
+  <si>
+    <t>stalk-surface-above-ring_y</t>
+  </si>
+  <si>
+    <t>stalk-surface-below-ring_f</t>
+  </si>
+  <si>
+    <t>stalk-surface-below-ring_k</t>
+  </si>
+  <si>
+    <t>stalk-surface-below-ring_s</t>
+  </si>
+  <si>
+    <t>stalk-surface-below-ring_y</t>
+  </si>
+  <si>
+    <t>stalk-color-above-ring_b</t>
+  </si>
+  <si>
+    <t>stalk-color-above-ring_c</t>
+  </si>
+  <si>
+    <t>stalk-color-above-ring_e</t>
+  </si>
+  <si>
+    <t>stalk-color-above-ring_g</t>
+  </si>
+  <si>
+    <t>stalk-color-above-ring_n</t>
+  </si>
+  <si>
+    <t>stalk-color-above-ring_o</t>
+  </si>
+  <si>
+    <t>stalk-color-above-ring_p</t>
+  </si>
+  <si>
+    <t>stalk-color-above-ring_w</t>
+  </si>
+  <si>
+    <t>stalk-color-above-ring_y</t>
+  </si>
+  <si>
+    <t>stalk-color-below-ring_b</t>
+  </si>
+  <si>
+    <t>stalk-color-below-ring_c</t>
+  </si>
+  <si>
+    <t>stalk-color-below-ring_e</t>
+  </si>
+  <si>
+    <t>stalk-color-below-ring_g</t>
+  </si>
+  <si>
+    <t>stalk-color-below-ring_n</t>
+  </si>
+  <si>
+    <t>stalk-color-below-ring_o</t>
+  </si>
+  <si>
+    <t>stalk-color-below-ring_p</t>
+  </si>
+  <si>
+    <t>stalk-color-below-ring_w</t>
+  </si>
+  <si>
+    <t>stalk-color-below-ring_y</t>
+  </si>
+  <si>
+    <t>veil-type_p</t>
+  </si>
+  <si>
+    <t>veil-color_n</t>
+  </si>
+  <si>
+    <t>veil-color_o</t>
+  </si>
+  <si>
+    <t>veil-color_w</t>
+  </si>
+  <si>
+    <t>veil-color_y</t>
+  </si>
+  <si>
+    <t>ring-number_n</t>
+  </si>
+  <si>
+    <t>ring-number_o</t>
+  </si>
+  <si>
+    <t>ring-number_t</t>
+  </si>
+  <si>
+    <t>ring-type_e</t>
+  </si>
+  <si>
+    <t>ring-type_f</t>
+  </si>
+  <si>
+    <t>ring-type_l</t>
+  </si>
+  <si>
+    <t>ring-type_n</t>
+  </si>
+  <si>
+    <t>ring-type_p</t>
+  </si>
+  <si>
+    <t>spore-print-color_b</t>
+  </si>
+  <si>
+    <t>spore-print-color_h</t>
+  </si>
+  <si>
+    <t>spore-print-color_k</t>
+  </si>
+  <si>
+    <t>spore-print-color_n</t>
+  </si>
+  <si>
+    <t>spore-print-color_o</t>
+  </si>
+  <si>
+    <t>spore-print-color_r</t>
+  </si>
+  <si>
+    <t>spore-print-color_u</t>
+  </si>
+  <si>
+    <t>spore-print-color_w</t>
+  </si>
+  <si>
+    <t>spore-print-color_y</t>
+  </si>
+  <si>
+    <t>population_a</t>
+  </si>
+  <si>
+    <t>population_c</t>
+  </si>
+  <si>
+    <t>population_n</t>
+  </si>
+  <si>
+    <t>population_s</t>
+  </si>
+  <si>
+    <t>population_v</t>
+  </si>
+  <si>
+    <t>population_y</t>
+  </si>
+  <si>
+    <t>habitat_d</t>
+  </si>
+  <si>
+    <t>habitat_g</t>
+  </si>
+  <si>
+    <t>habitat_l</t>
+  </si>
+  <si>
+    <t>habitat_m</t>
+  </si>
+  <si>
+    <t>habitat_p</t>
+  </si>
+  <si>
+    <t>habitat_u</t>
+  </si>
+  <si>
+    <t>habitat_w</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -96,6 +546,22 @@
     <font>
       <b/>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -137,7 +603,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -148,6 +614,13 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -164,6 +637,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="logreg_coef" connectionId="1" xr16:uid="{EF66FBA7-5501-D84E-A51C-5E69935DA11D}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -465,7 +942,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0527CFA8-2165-904B-95B1-83656C2273CB}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:C9"/>
     </sheetView>
   </sheetViews>
@@ -559,4 +1036,1175 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F54BDCB8-D80B-D048-B4FF-1A5A94A96E68}">
+  <dimension ref="A1:H8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.83203125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="23" style="6" customWidth="1"/>
+    <col min="3" max="4" width="26.33203125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" s="7">
+        <v>0</v>
+      </c>
+      <c r="H2" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{726BD5E2-0E01-8F4F-A14A-7E9F2D22E84B}">
+  <dimension ref="A1:F118"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.33203125" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2">
+        <v>4.0642681511831302</v>
+      </c>
+      <c r="E2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F2">
+        <v>4.0642681511831302</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3">
+        <v>2.6561329702418801</v>
+      </c>
+      <c r="E3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F3">
+        <v>2.6561329702418801</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4">
+        <v>2.6467145361152</v>
+      </c>
+      <c r="E4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F4">
+        <v>2.6467145361152</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5">
+        <v>1.9590787966176499</v>
+      </c>
+      <c r="E5" t="s">
+        <v>80</v>
+      </c>
+      <c r="F5">
+        <v>1.9590787966176499</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>143</v>
+      </c>
+      <c r="B6">
+        <v>1.4567768076274901</v>
+      </c>
+      <c r="E6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F6">
+        <v>-1.52187927724365</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>136</v>
+      </c>
+      <c r="B7">
+        <v>1.4549139905217701</v>
+      </c>
+      <c r="E7" t="s">
+        <v>102</v>
+      </c>
+      <c r="F7">
+        <v>-1.6653358756119701</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B8">
+        <v>1.4139893973371001</v>
+      </c>
+      <c r="E8" t="s">
+        <v>82</v>
+      </c>
+      <c r="F8">
+        <v>-1.79892937718296</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>146</v>
+      </c>
+      <c r="B9">
+        <v>1.3523577572299299</v>
+      </c>
+      <c r="E9" t="s">
+        <v>81</v>
+      </c>
+      <c r="F9">
+        <v>-2.0669686765241999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>142</v>
+      </c>
+      <c r="B10">
+        <v>1.3000365123069699</v>
+      </c>
+      <c r="E10" t="s">
+        <v>73</v>
+      </c>
+      <c r="F10">
+        <v>-2.2525941321962799</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>154</v>
+      </c>
+      <c r="B11">
+        <v>1.08639866057423</v>
+      </c>
+      <c r="E11" t="s">
+        <v>97</v>
+      </c>
+      <c r="F11">
+        <v>-2.2865990544670098</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>161</v>
+      </c>
+      <c r="B12">
+        <v>1.06671966923178</v>
+      </c>
+      <c r="E12" t="s">
+        <v>69</v>
+      </c>
+      <c r="F12">
+        <v>-2.6077306416235202</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>103</v>
+      </c>
+      <c r="B13">
+        <v>1.0409138521498</v>
+      </c>
+      <c r="E13" t="s">
+        <v>68</v>
+      </c>
+      <c r="F13">
+        <v>-2.6383606862846301</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>105</v>
+      </c>
+      <c r="B14">
+        <v>1.0259801274485401</v>
+      </c>
+      <c r="E14" t="s">
+        <v>145</v>
+      </c>
+      <c r="F14">
+        <v>-3.3305637545492899</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>98</v>
+      </c>
+      <c r="B15">
+        <v>0.93366195133963503</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>122</v>
+      </c>
+      <c r="B16">
+        <v>0.88683442264871004</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>100</v>
+      </c>
+      <c r="B17">
+        <v>0.87989663018523601</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18">
+        <v>0.82789148887396902</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>151</v>
+      </c>
+      <c r="B19">
+        <v>0.74851967181207502</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20">
+        <v>0.67653259338859095</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>101</v>
+      </c>
+      <c r="B21">
+        <v>0.64490179794124103</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>87</v>
+      </c>
+      <c r="B22">
+        <v>0.61573271189922296</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>95</v>
+      </c>
+      <c r="B23">
+        <v>0.55519878173708304</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>83</v>
+      </c>
+      <c r="B24">
+        <v>0.53170559818956897</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25">
+        <v>0.51727696877347995</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>96</v>
+      </c>
+      <c r="B26">
+        <v>0.49604564051688799</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>107</v>
+      </c>
+      <c r="B27">
+        <v>0.47385658848509299</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>89</v>
+      </c>
+      <c r="B28">
+        <v>0.43936380897055199</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>92</v>
+      </c>
+      <c r="B29">
+        <v>0.42046455082328299</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>111</v>
+      </c>
+      <c r="B30">
+        <v>0.40542847195690002</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>86</v>
+      </c>
+      <c r="B31">
+        <v>0.40369992173798802</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>112</v>
+      </c>
+      <c r="B32">
+        <v>0.35473497379792202</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>120</v>
+      </c>
+      <c r="B33">
+        <v>0.35046517699729801</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>159</v>
+      </c>
+      <c r="B34">
+        <v>0.34211357295803102</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>62</v>
+      </c>
+      <c r="B35">
+        <v>0.33870644237159098</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>59</v>
+      </c>
+      <c r="B36">
+        <v>0.33158054188338498</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>61</v>
+      </c>
+      <c r="B37">
+        <v>0.32574536374456797</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>121</v>
+      </c>
+      <c r="B38">
+        <v>0.323253332772799</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>114</v>
+      </c>
+      <c r="B39">
+        <v>0.27574200605313998</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>123</v>
+      </c>
+      <c r="B40">
+        <v>0.27574200605313998</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>155</v>
+      </c>
+      <c r="B41">
+        <v>0.27161859043473102</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>64</v>
+      </c>
+      <c r="B42">
+        <v>0.25972976627558497</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>50</v>
+      </c>
+      <c r="B43">
+        <v>0.21203187612947999</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>91</v>
+      </c>
+      <c r="B44">
+        <v>0.20886386370052001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>130</v>
+      </c>
+      <c r="B45">
+        <v>0.20776717732696301</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>113</v>
+      </c>
+      <c r="B46">
+        <v>0.18459830553435999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>47</v>
+      </c>
+      <c r="B47">
+        <v>0.16523295419852399</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>129</v>
+      </c>
+      <c r="B48">
+        <v>0.145060259569956</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>134</v>
+      </c>
+      <c r="B49">
+        <v>0.14004576506525501</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>139</v>
+      </c>
+      <c r="B50">
+        <v>0.13400161791212001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>128</v>
+      </c>
+      <c r="B51">
+        <v>0.13068174648318401</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>76</v>
+      </c>
+      <c r="B52">
+        <v>9.7300980053514993E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>140</v>
+      </c>
+      <c r="B53">
+        <v>9.0852377989306496E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>88</v>
+      </c>
+      <c r="B54">
+        <v>8.9693886706088799E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>144</v>
+      </c>
+      <c r="B55">
+        <v>8.9593637004715898E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>133</v>
+      </c>
+      <c r="B56">
+        <v>7.9323217723809195E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>148</v>
+      </c>
+      <c r="B57">
+        <v>7.1404075195050695E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>116</v>
+      </c>
+      <c r="B58">
+        <v>4.3875625354557801E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>149</v>
+      </c>
+      <c r="B59">
+        <v>1.5860446208406199E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>65</v>
+      </c>
+      <c r="B60">
+        <v>3.2378272816936502E-3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>84</v>
+      </c>
+      <c r="B61">
+        <v>-2.0075415181985901E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>57</v>
+      </c>
+      <c r="B62">
+        <v>-2.6949371507277099E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>54</v>
+      </c>
+      <c r="B63">
+        <v>-2.9028928428815898E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>157</v>
+      </c>
+      <c r="B64">
+        <v>-3.3062436300158697E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>85</v>
+      </c>
+      <c r="B65">
+        <v>-3.8335842857781501E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>58</v>
+      </c>
+      <c r="B66">
+        <v>-3.89641436790477E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>127</v>
+      </c>
+      <c r="B67">
+        <v>-0.107889879906566</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>66</v>
+      </c>
+      <c r="B68">
+        <v>-0.11112770718824801</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>104</v>
+      </c>
+      <c r="B69">
+        <v>-0.128369654385633</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>99</v>
+      </c>
+      <c r="B70">
+        <v>-0.13089504748132999</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>147</v>
+      </c>
+      <c r="B71">
+        <v>-0.13539880414525199</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>118</v>
+      </c>
+      <c r="B72">
+        <v>-0.136389166745637</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>48</v>
+      </c>
+      <c r="B73">
+        <v>-0.17494808496604899</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>109</v>
+      </c>
+      <c r="B74">
+        <v>-0.18349409690042201</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>77</v>
+      </c>
+      <c r="B75">
+        <v>-0.20519085996005801</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>45</v>
+      </c>
+      <c r="B76">
+        <v>-0.253656587766736</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>115</v>
+      </c>
+      <c r="B77">
+        <v>-0.270117239720711</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>125</v>
+      </c>
+      <c r="B78">
+        <v>-0.27672174417342399</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>93</v>
+      </c>
+      <c r="B79">
+        <v>-0.29495194073060699</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>53</v>
+      </c>
+      <c r="B80">
+        <v>-0.30841198459200297</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>160</v>
+      </c>
+      <c r="B81">
+        <v>-0.32074252780664297</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>71</v>
+      </c>
+      <c r="B82">
+        <v>-0.32725886269564303</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>110</v>
+      </c>
+      <c r="B83">
+        <v>-0.32725886269564303</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>119</v>
+      </c>
+      <c r="B84">
+        <v>-0.32725886269564303</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>132</v>
+      </c>
+      <c r="B85">
+        <v>-0.32725886269564303</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>138</v>
+      </c>
+      <c r="B86">
+        <v>-0.32725886269564303</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>124</v>
+      </c>
+      <c r="B87">
+        <v>-0.344573260710764</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>63</v>
+      </c>
+      <c r="B88">
+        <v>-0.359006791640259</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>106</v>
+      </c>
+      <c r="B89">
+        <v>-0.39534640882383898</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>153</v>
+      </c>
+      <c r="B90">
+        <v>-0.41273167983943498</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>152</v>
+      </c>
+      <c r="B91">
+        <v>-0.41962708691930301</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>52</v>
+      </c>
+      <c r="B92">
+        <v>-0.44698156027434299</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>46</v>
+      </c>
+      <c r="B93">
+        <v>-0.57382700627527705</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>117</v>
+      </c>
+      <c r="B94">
+        <v>-0.59139906328665004</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>131</v>
+      </c>
+      <c r="B95">
+        <v>-0.59139906328665004</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>137</v>
+      </c>
+      <c r="B96">
+        <v>-0.64516377938238201</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>94</v>
+      </c>
+      <c r="B97">
+        <v>-0.663088661643643</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>90</v>
+      </c>
+      <c r="B98">
+        <v>-0.66512164598045997</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>156</v>
+      </c>
+      <c r="B99">
+        <v>-0.67861576375741095</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>135</v>
+      </c>
+      <c r="B100">
+        <v>-0.72438284626244198</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>158</v>
+      </c>
+      <c r="B101">
+        <v>-0.75592098466690705</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>75</v>
+      </c>
+      <c r="B102">
+        <v>-0.803014748916831</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>60</v>
+      </c>
+      <c r="B103">
+        <v>-0.83970055518478603</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>74</v>
+      </c>
+      <c r="B104">
+        <v>-0.84604646572987197</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>126</v>
+      </c>
+      <c r="B105">
+        <v>-0.85924178405303298</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>55</v>
+      </c>
+      <c r="B106">
+        <v>-0.92692262104429501</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>141</v>
+      </c>
+      <c r="B107">
+        <v>-1.00294848856549</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>150</v>
+      </c>
+      <c r="B108">
+        <v>-1.12630989174254</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>108</v>
+      </c>
+      <c r="B109">
+        <v>-1.21238018701636</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>78</v>
+      </c>
+      <c r="B110">
+        <v>-1.52187927724365</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>102</v>
+      </c>
+      <c r="B111">
+        <v>-1.6653358756119701</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>82</v>
+      </c>
+      <c r="B112">
+        <v>-1.79892937718296</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>81</v>
+      </c>
+      <c r="B113">
+        <v>-2.0669686765241999</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>73</v>
+      </c>
+      <c r="B114">
+        <v>-2.2525941321962799</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>97</v>
+      </c>
+      <c r="B115">
+        <v>-2.2865990544670098</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>69</v>
+      </c>
+      <c r="B116">
+        <v>-2.6077306416235202</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>68</v>
+      </c>
+      <c r="B117">
+        <v>-2.6383606862846301</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>145</v>
+      </c>
+      <c r="B118">
+        <v>-3.3305637545492899</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="E2:F14">
+    <sortCondition descending="1" ref="F2:F14"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>